<commit_message>
code and ppt uploaded
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiranjeev\Documents\Investment case study Cohort-3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -17,11 +12,8 @@
     <sheet name="Table-3.1" sheetId="5" r:id="rId3"/>
     <sheet name="Table-5.1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -33,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>C1</t>
   </si>
@@ -357,12 +349,72 @@
   </si>
   <si>
     <t>Sector-wise Investment Analysis</t>
+  </si>
+  <si>
+    <t>permalink</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> United States</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Social, Finance, Analytics, Advertising</t>
+  </si>
+  <si>
+    <t>Cleantech / Semiconductors</t>
+  </si>
+  <si>
+    <t>News, Search and Messaging</t>
+  </si>
+  <si>
+    <t>Electric Cloud</t>
+  </si>
+  <si>
+    <t>SST Inc. (Formerly ShotSpotter)</t>
+  </si>
+  <si>
+    <t>11724223  USD</t>
+  </si>
+  <si>
+    <t>971575 USD</t>
+  </si>
+  <si>
+    <t>747793 USD</t>
+  </si>
+  <si>
+    <t>73938484 USD</t>
+  </si>
+  <si>
+    <t>Virtustream</t>
+  </si>
+  <si>
+    <t>FirstCry.com</t>
+  </si>
+  <si>
+    <t>Celltick Technologies</t>
+  </si>
+  <si>
+    <t>Manthan Systems</t>
+  </si>
+  <si>
+    <t>Venture investment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -632,48 +684,49 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,7 +1033,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -990,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,23 +1055,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1038,7 +1091,9 @@
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17">
+        <v>66370</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1047,7 +1102,9 @@
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="17">
+        <v>66368</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -1056,7 +1113,9 @@
       <c r="B7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1065,7 +1124,9 @@
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1074,7 +1135,9 @@
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="17">
+        <v>114942</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
@@ -1106,7 +1169,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,21 +1180,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1151,7 +1214,9 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -1160,7 +1225,9 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
@@ -1169,7 +1236,9 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -1178,7 +1247,9 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -1187,7 +1258,9 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1214,7 +1287,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,21 +1298,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1259,7 +1332,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1268,7 +1343,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -1277,7 +1354,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1302,52 +1381,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="56.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="4" max="5" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="24" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1358,9 +1436,15 @@
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="C5" s="17">
+        <v>12092</v>
+      </c>
+      <c r="D5" s="17">
+        <v>622</v>
+      </c>
+      <c r="E5" s="17">
+        <v>328</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
@@ -1369,9 +1453,15 @@
       <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="36">
+        <v>108002096957</v>
+      </c>
+      <c r="D6" s="17">
+        <v>5394078692</v>
+      </c>
+      <c r="E6" s="17">
+        <v>2949543602</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
@@ -1380,9 +1470,15 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
@@ -1391,9 +1487,15 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
@@ -1402,9 +1504,15 @@
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
@@ -1413,9 +1521,15 @@
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="17">
+        <v>2957</v>
+      </c>
+      <c r="D10" s="17">
+        <v>148</v>
+      </c>
+      <c r="E10" s="17">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
@@ -1424,9 +1538,15 @@
       <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="17">
+        <v>2718</v>
+      </c>
+      <c r="D11" s="17">
+        <v>133</v>
+      </c>
+      <c r="E11" s="17">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
@@ -1435,9 +1555,15 @@
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="17">
+        <v>2355</v>
+      </c>
+      <c r="D12" s="17">
+        <v>130</v>
+      </c>
+      <c r="E12" s="17">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
@@ -1446,9 +1572,15 @@
       <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
@@ -1457,9 +1589,15 @@
       <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>